<commit_message>
Created the shop.cs for printing out all products and add products to the shopping cart. Created basic entities for shoppingcart and shoppingcartitem.
Created also a method for add products to shopping cart in shoppingcartservice.

Closes #13
</commit_message>
<xml_diff>
--- a/ToDo-Planung_Heydemann_Daehne_Bechtel_Hörnchen.xlsx
+++ b/ToDo-Planung_Heydemann_Daehne_Bechtel_Hörnchen.xlsx
@@ -665,7 +665,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,9 +859,11 @@
         <v>120</v>
       </c>
       <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1359,18 +1361,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1392,14 +1394,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{353EF643-0AB6-4413-8F22-D5DFD2ED6691}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12A48405-2C1B-401F-8245-98D10AB601AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1413,4 +1407,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{353EF643-0AB6-4413-8F22-D5DFD2ED6691}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Kompletten Shop und angefangen den Einkaufswagen und den Abschluss zu machen
</commit_message>
<xml_diff>
--- a/ToDo-Planung_Heydemann_Daehne_Bechtel_Hörnchen.xlsx
+++ b/ToDo-Planung_Heydemann_Daehne_Bechtel_Hörnchen.xlsx
@@ -665,7 +665,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,18 +1361,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1394,6 +1394,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{353EF643-0AB6-4413-8F22-D5DFD2ED6691}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12A48405-2C1B-401F-8245-98D10AB601AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1407,12 +1415,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{353EF643-0AB6-4413-8F22-D5DFD2ED6691}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>